<commit_message>
Block Rush QA changes done
</commit_message>
<xml_diff>
--- a/Plug In Digital/blockrush/Guidelines Android France Block Rush.xlsx
+++ b/Plug In Digital/blockrush/Guidelines Android France Block Rush.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Other Coding\WebApps\artridge\Plug In Digital\blockrush\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5272271D-AB2F-428A-8A9F-DC56FE9FA232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA5CBC7-78F8-4940-9AE6-B3AD92894C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A005AC79-4D67-46D0-B597-4CE960B40E81}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A005AC79-4D67-46D0-B597-4CE960B40E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadatas" sheetId="1" r:id="rId1"/>
@@ -571,6 +571,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -587,28 +614,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -620,15 +625,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -638,27 +634,31 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -975,7 +975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB8EC11B-37B5-4B46-8BC2-A20FF7AB1A3B}">
   <dimension ref="B1:P74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B74" sqref="B74:G74"/>
     </sheetView>
   </sheetViews>
@@ -985,22 +985,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="58"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="46"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="48"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="37"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
@@ -1014,21 +1014,21 @@
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="31"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="40"/>
     </row>
     <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="34"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="43"/>
     </row>
     <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
@@ -1042,21 +1042,21 @@
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="31"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="40"/>
     </row>
     <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="34"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="43"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
@@ -1067,22 +1067,22 @@
       <c r="G9" s="8"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="46"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="46"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="48"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="37"/>
     </row>
     <row r="12" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
@@ -1096,13 +1096,13 @@
       <c r="B13" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="52" t="s">
+      <c r="C13" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="54"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="31"/>
     </row>
     <row r="14" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
@@ -1116,33 +1116,33 @@
       <c r="B15" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="52" t="s">
+      <c r="C15" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="54"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="31"/>
     </row>
     <row r="16" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="49"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="51"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="49"/>
     </row>
     <row r="17" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="52" t="s">
+      <c r="C17" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="54"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="31"/>
     </row>
     <row r="18" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
@@ -1156,13 +1156,13 @@
       <c r="B19" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="52" t="s">
+      <c r="C19" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="54"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="31"/>
     </row>
     <row r="20" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
@@ -1176,13 +1176,13 @@
       <c r="B21" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="52" t="s">
+      <c r="C21" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="54"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="31"/>
     </row>
     <row r="22" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
@@ -1196,13 +1196,13 @@
       <c r="B23" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="52" t="s">
+      <c r="C23" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="54"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="31"/>
     </row>
     <row r="24" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
@@ -1218,21 +1218,21 @@
       <c r="B25" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="31"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="40"/>
     </row>
     <row r="26" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="34"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="43"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
@@ -1243,50 +1243,50 @@
       <c r="G27" s="6"/>
     </row>
     <row r="28" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="43" t="s">
+      <c r="B28" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="46"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="46"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="48"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="37"/>
     </row>
     <row r="30" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="55"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="50"/>
-      <c r="G30" s="51"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="49"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="29" t="s">
+      <c r="C31" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="31"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="40"/>
     </row>
     <row r="32" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="34"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="43"/>
     </row>
     <row r="33" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
@@ -1300,21 +1300,21 @@
       <c r="B34" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C34" s="29" t="s">
+      <c r="C34" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="31"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="40"/>
     </row>
     <row r="35" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="34"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="42"/>
+      <c r="G35" s="43"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
@@ -1325,22 +1325,22 @@
       <c r="G36" s="6"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="43" t="s">
+      <c r="B37" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="45"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="46"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="46"/>
-      <c r="C38" s="47"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="48"/>
+      <c r="B38" s="35"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="37"/>
     </row>
     <row r="39" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
@@ -1354,21 +1354,21 @@
       <c r="B40" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C40" s="29" t="s">
+      <c r="C40" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="30"/>
-      <c r="G40" s="31"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="39"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="40"/>
     </row>
     <row r="41" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="34"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="43"/>
     </row>
     <row r="42" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
@@ -1382,308 +1382,324 @@
       <c r="B43" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C43" s="29" t="s">
+      <c r="C43" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="D43" s="30"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="30"/>
-      <c r="G43" s="31"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="40"/>
     </row>
     <row r="44" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>
-      <c r="C44" s="32"/>
-      <c r="D44" s="33"/>
-      <c r="E44" s="33"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="34"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="42"/>
+      <c r="G44" s="43"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="40"/>
-      <c r="C45" s="41"/>
-      <c r="D45" s="41"/>
-      <c r="E45" s="41"/>
-      <c r="F45" s="41"/>
-      <c r="G45" s="42"/>
+      <c r="B45" s="51"/>
+      <c r="C45" s="52"/>
+      <c r="D45" s="52"/>
+      <c r="E45" s="52"/>
+      <c r="F45" s="52"/>
+      <c r="G45" s="53"/>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="43" t="s">
+      <c r="B46" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="C46" s="44"/>
-      <c r="D46" s="44"/>
-      <c r="E46" s="44"/>
-      <c r="F46" s="44"/>
-      <c r="G46" s="45"/>
+      <c r="C46" s="45"/>
+      <c r="D46" s="45"/>
+      <c r="E46" s="45"/>
+      <c r="F46" s="45"/>
+      <c r="G46" s="46"/>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="46"/>
-      <c r="C47" s="47"/>
-      <c r="D47" s="47"/>
-      <c r="E47" s="47"/>
-      <c r="F47" s="47"/>
-      <c r="G47" s="48"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="37"/>
     </row>
     <row r="48" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="40"/>
-      <c r="C48" s="41"/>
-      <c r="D48" s="41"/>
-      <c r="E48" s="41"/>
-      <c r="F48" s="41"/>
-      <c r="G48" s="42"/>
+      <c r="B48" s="51"/>
+      <c r="C48" s="52"/>
+      <c r="D48" s="52"/>
+      <c r="E48" s="52"/>
+      <c r="F48" s="52"/>
+      <c r="G48" s="53"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C49" s="29" t="s">
+      <c r="C49" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="30"/>
-      <c r="G49" s="31"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="39"/>
+      <c r="F49" s="39"/>
+      <c r="G49" s="40"/>
     </row>
     <row r="50" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="1"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="33"/>
-      <c r="E50" s="33"/>
-      <c r="F50" s="33"/>
-      <c r="G50" s="34"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="42"/>
+      <c r="E50" s="42"/>
+      <c r="F50" s="42"/>
+      <c r="G50" s="43"/>
     </row>
     <row r="51" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="40"/>
-      <c r="C51" s="41"/>
-      <c r="D51" s="41"/>
-      <c r="E51" s="41"/>
-      <c r="F51" s="41"/>
-      <c r="G51" s="42"/>
+      <c r="B51" s="51"/>
+      <c r="C51" s="52"/>
+      <c r="D51" s="52"/>
+      <c r="E51" s="52"/>
+      <c r="F51" s="52"/>
+      <c r="G51" s="53"/>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B52" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C52" s="29" t="s">
+      <c r="C52" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="D52" s="30"/>
-      <c r="E52" s="30"/>
-      <c r="F52" s="30"/>
-      <c r="G52" s="31"/>
+      <c r="D52" s="39"/>
+      <c r="E52" s="39"/>
+      <c r="F52" s="39"/>
+      <c r="G52" s="40"/>
     </row>
     <row r="53" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="1"/>
-      <c r="C53" s="32"/>
-      <c r="D53" s="33"/>
-      <c r="E53" s="33"/>
-      <c r="F53" s="33"/>
-      <c r="G53" s="34"/>
+      <c r="C53" s="41"/>
+      <c r="D53" s="42"/>
+      <c r="E53" s="42"/>
+      <c r="F53" s="42"/>
+      <c r="G53" s="43"/>
     </row>
     <row r="54" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="40"/>
-      <c r="C54" s="41"/>
-      <c r="D54" s="41"/>
-      <c r="E54" s="41"/>
-      <c r="F54" s="41"/>
-      <c r="G54" s="42"/>
+      <c r="B54" s="51"/>
+      <c r="C54" s="52"/>
+      <c r="D54" s="52"/>
+      <c r="E54" s="52"/>
+      <c r="F54" s="52"/>
+      <c r="G54" s="53"/>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C55" s="29" t="s">
+      <c r="C55" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="D55" s="30"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="30"/>
-      <c r="G55" s="31"/>
+      <c r="D55" s="39"/>
+      <c r="E55" s="39"/>
+      <c r="F55" s="39"/>
+      <c r="G55" s="40"/>
     </row>
     <row r="56" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="1"/>
-      <c r="C56" s="32"/>
-      <c r="D56" s="33"/>
-      <c r="E56" s="33"/>
-      <c r="F56" s="33"/>
-      <c r="G56" s="34"/>
+      <c r="C56" s="41"/>
+      <c r="D56" s="42"/>
+      <c r="E56" s="42"/>
+      <c r="F56" s="42"/>
+      <c r="G56" s="43"/>
     </row>
     <row r="57" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="40"/>
-      <c r="C57" s="41"/>
-      <c r="D57" s="41"/>
-      <c r="E57" s="41"/>
-      <c r="F57" s="41"/>
-      <c r="G57" s="42"/>
+      <c r="B57" s="51"/>
+      <c r="C57" s="52"/>
+      <c r="D57" s="52"/>
+      <c r="E57" s="52"/>
+      <c r="F57" s="52"/>
+      <c r="G57" s="53"/>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B58" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C58" s="29" t="s">
+      <c r="C58" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="D58" s="30"/>
-      <c r="E58" s="30"/>
-      <c r="F58" s="30"/>
-      <c r="G58" s="31"/>
+      <c r="D58" s="39"/>
+      <c r="E58" s="39"/>
+      <c r="F58" s="39"/>
+      <c r="G58" s="40"/>
     </row>
     <row r="59" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="1"/>
-      <c r="C59" s="32"/>
-      <c r="D59" s="33"/>
-      <c r="E59" s="33"/>
-      <c r="F59" s="33"/>
-      <c r="G59" s="34"/>
+      <c r="C59" s="41"/>
+      <c r="D59" s="42"/>
+      <c r="E59" s="42"/>
+      <c r="F59" s="42"/>
+      <c r="G59" s="43"/>
     </row>
     <row r="60" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="40"/>
-      <c r="C60" s="41"/>
-      <c r="D60" s="41"/>
-      <c r="E60" s="41"/>
-      <c r="F60" s="41"/>
-      <c r="G60" s="42"/>
+      <c r="B60" s="51"/>
+      <c r="C60" s="52"/>
+      <c r="D60" s="52"/>
+      <c r="E60" s="52"/>
+      <c r="F60" s="52"/>
+      <c r="G60" s="53"/>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B61" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C61" s="29" t="s">
+      <c r="C61" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D61" s="30"/>
-      <c r="E61" s="30"/>
-      <c r="F61" s="30"/>
-      <c r="G61" s="31"/>
+      <c r="D61" s="39"/>
+      <c r="E61" s="39"/>
+      <c r="F61" s="39"/>
+      <c r="G61" s="40"/>
     </row>
     <row r="62" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="1"/>
-      <c r="C62" s="32"/>
-      <c r="D62" s="33"/>
-      <c r="E62" s="33"/>
-      <c r="F62" s="33"/>
-      <c r="G62" s="34"/>
+      <c r="C62" s="41"/>
+      <c r="D62" s="42"/>
+      <c r="E62" s="42"/>
+      <c r="F62" s="42"/>
+      <c r="G62" s="43"/>
     </row>
     <row r="63" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="40"/>
-      <c r="C63" s="41"/>
-      <c r="D63" s="41"/>
-      <c r="E63" s="41"/>
-      <c r="F63" s="41"/>
-      <c r="G63" s="42"/>
+      <c r="B63" s="51"/>
+      <c r="C63" s="52"/>
+      <c r="D63" s="52"/>
+      <c r="E63" s="52"/>
+      <c r="F63" s="52"/>
+      <c r="G63" s="53"/>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B64" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C64" s="29" t="s">
+      <c r="C64" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="D64" s="30"/>
-      <c r="E64" s="30"/>
-      <c r="F64" s="30"/>
-      <c r="G64" s="31"/>
+      <c r="D64" s="39"/>
+      <c r="E64" s="39"/>
+      <c r="F64" s="39"/>
+      <c r="G64" s="40"/>
     </row>
     <row r="65" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="1"/>
-      <c r="C65" s="32"/>
-      <c r="D65" s="33"/>
-      <c r="E65" s="33"/>
-      <c r="F65" s="33"/>
-      <c r="G65" s="34"/>
+      <c r="C65" s="41"/>
+      <c r="D65" s="42"/>
+      <c r="E65" s="42"/>
+      <c r="F65" s="42"/>
+      <c r="G65" s="43"/>
     </row>
     <row r="66" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="40"/>
-      <c r="C66" s="41"/>
-      <c r="D66" s="41"/>
-      <c r="E66" s="41"/>
-      <c r="F66" s="41"/>
-      <c r="G66" s="42"/>
+      <c r="B66" s="51"/>
+      <c r="C66" s="52"/>
+      <c r="D66" s="52"/>
+      <c r="E66" s="52"/>
+      <c r="F66" s="52"/>
+      <c r="G66" s="53"/>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C67" s="38" t="s">
+      <c r="C67" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D67" s="30"/>
-      <c r="E67" s="30"/>
-      <c r="F67" s="30"/>
-      <c r="G67" s="31"/>
+      <c r="D67" s="39"/>
+      <c r="E67" s="39"/>
+      <c r="F67" s="39"/>
+      <c r="G67" s="40"/>
     </row>
     <row r="68" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="1"/>
-      <c r="C68" s="32"/>
-      <c r="D68" s="33"/>
-      <c r="E68" s="33"/>
-      <c r="F68" s="33"/>
-      <c r="G68" s="34"/>
+      <c r="C68" s="41"/>
+      <c r="D68" s="42"/>
+      <c r="E68" s="42"/>
+      <c r="F68" s="42"/>
+      <c r="G68" s="43"/>
     </row>
     <row r="69" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="40"/>
-      <c r="C69" s="41"/>
-      <c r="D69" s="41"/>
-      <c r="E69" s="41"/>
-      <c r="F69" s="41"/>
-      <c r="G69" s="42"/>
+      <c r="B69" s="51"/>
+      <c r="C69" s="52"/>
+      <c r="D69" s="52"/>
+      <c r="E69" s="52"/>
+      <c r="F69" s="52"/>
+      <c r="G69" s="53"/>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B70" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C70" s="29">
+      <c r="C70" s="38">
         <v>2.11</v>
       </c>
-      <c r="D70" s="30"/>
-      <c r="E70" s="30"/>
-      <c r="F70" s="30"/>
-      <c r="G70" s="31"/>
+      <c r="D70" s="39"/>
+      <c r="E70" s="39"/>
+      <c r="F70" s="39"/>
+      <c r="G70" s="40"/>
     </row>
     <row r="71" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="1"/>
-      <c r="C71" s="32"/>
-      <c r="D71" s="33"/>
-      <c r="E71" s="33"/>
-      <c r="F71" s="33"/>
-      <c r="G71" s="34"/>
+      <c r="C71" s="41"/>
+      <c r="D71" s="42"/>
+      <c r="E71" s="42"/>
+      <c r="F71" s="42"/>
+      <c r="G71" s="43"/>
     </row>
     <row r="72" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="35"/>
-      <c r="C72" s="36"/>
-      <c r="D72" s="36"/>
-      <c r="E72" s="36"/>
-      <c r="F72" s="36"/>
-      <c r="G72" s="37"/>
+      <c r="B72" s="54"/>
+      <c r="C72" s="55"/>
+      <c r="D72" s="55"/>
+      <c r="E72" s="55"/>
+      <c r="F72" s="55"/>
+      <c r="G72" s="56"/>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B73" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C73" s="38" t="s">
+      <c r="C73" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D73" s="39"/>
-      <c r="E73" s="39"/>
-      <c r="F73" s="39"/>
-      <c r="G73" s="39"/>
+      <c r="D73" s="58"/>
+      <c r="E73" s="58"/>
+      <c r="F73" s="58"/>
+      <c r="G73" s="58"/>
     </row>
     <row r="74" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="35"/>
-      <c r="C74" s="36"/>
-      <c r="D74" s="36"/>
-      <c r="E74" s="36"/>
-      <c r="F74" s="36"/>
-      <c r="G74" s="37"/>
+      <c r="B74" s="54"/>
+      <c r="C74" s="55"/>
+      <c r="D74" s="55"/>
+      <c r="E74" s="55"/>
+      <c r="F74" s="55"/>
+      <c r="G74" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="B1:G2"/>
-    <mergeCell ref="C4:G5"/>
-    <mergeCell ref="C7:G8"/>
-    <mergeCell ref="B10:G11"/>
-    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C70:G71"/>
+    <mergeCell ref="B72:G72"/>
+    <mergeCell ref="C73:G73"/>
+    <mergeCell ref="B74:G74"/>
+    <mergeCell ref="C61:G62"/>
+    <mergeCell ref="B63:G63"/>
+    <mergeCell ref="C64:G65"/>
+    <mergeCell ref="B66:G66"/>
+    <mergeCell ref="C67:G68"/>
+    <mergeCell ref="B69:G69"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="C43:G44"/>
+    <mergeCell ref="B45:G45"/>
+    <mergeCell ref="B46:G47"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="C49:G50"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="C52:G53"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="C55:G56"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="C58:G59"/>
     <mergeCell ref="C40:G41"/>
     <mergeCell ref="B16:G16"/>
     <mergeCell ref="C17:G17"/>
@@ -1696,28 +1712,12 @@
     <mergeCell ref="C31:G32"/>
     <mergeCell ref="C34:G35"/>
     <mergeCell ref="B37:G38"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="C43:G44"/>
-    <mergeCell ref="B45:G45"/>
-    <mergeCell ref="B46:G47"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="C49:G50"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="C52:G53"/>
-    <mergeCell ref="B54:G54"/>
-    <mergeCell ref="C55:G56"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="C58:G59"/>
-    <mergeCell ref="C70:G71"/>
-    <mergeCell ref="B72:G72"/>
-    <mergeCell ref="C73:G73"/>
-    <mergeCell ref="B74:G74"/>
-    <mergeCell ref="C61:G62"/>
-    <mergeCell ref="B63:G63"/>
-    <mergeCell ref="C64:G65"/>
-    <mergeCell ref="B66:G66"/>
-    <mergeCell ref="C67:G68"/>
-    <mergeCell ref="B69:G69"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="B1:G2"/>
+    <mergeCell ref="C4:G5"/>
+    <mergeCell ref="C7:G8"/>
+    <mergeCell ref="B10:G11"/>
+    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -1728,8 +1728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F40B79FA-81E3-4B65-BD43-437DAC09E605}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1882,12 +1882,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2094,15 +2091,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7B463CC-2C6E-4AEC-AFE4-31056C900892}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9798A1B8-6B7D-4E6C-A31B-78AFC6E86C13}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="0b7efa9e-1eed-4bd4-901e-1ea14744ffa0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="d82d40c8-bfdf-4ce1-b1ad-6594fbc9adc4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2127,18 +2136,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9798A1B8-6B7D-4E6C-A31B-78AFC6E86C13}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7B463CC-2C6E-4AEC-AFE4-31056C900892}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="0b7efa9e-1eed-4bd4-901e-1ea14744ffa0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="d82d40c8-bfdf-4ce1-b1ad-6594fbc9adc4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
QA testing changes all done
</commit_message>
<xml_diff>
--- a/Plug In Digital/blockrush/Guidelines Android France Block Rush.xlsx
+++ b/Plug In Digital/blockrush/Guidelines Android France Block Rush.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Other Coding\WebApps\artridge\Plug In Digital\blockrush\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA5CBC7-78F8-4940-9AE6-B3AD92894C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C7C5A9-AB95-4EC1-9A6C-3A0B23257530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A005AC79-4D67-46D0-B597-4CE960B40E81}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A005AC79-4D67-46D0-B597-4CE960B40E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadatas" sheetId="1" r:id="rId1"/>
@@ -571,6 +571,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -578,6 +645,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -589,76 +659,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -975,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB8EC11B-37B5-4B46-8BC2-A20FF7AB1A3B}">
   <dimension ref="B1:P74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B74" sqref="B74:G74"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72:G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,22 +985,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="34"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="58"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="35"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="37"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="48"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
@@ -1014,21 +1014,21 @@
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="40"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="31"/>
     </row>
     <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="43"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="34"/>
     </row>
     <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
@@ -1042,21 +1042,21 @@
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="40"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="31"/>
     </row>
     <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="43"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="34"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
@@ -1067,22 +1067,22 @@
       <c r="G9" s="8"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="46"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="45"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="37"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="48"/>
     </row>
     <row r="12" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
@@ -1096,13 +1096,13 @@
       <c r="B13" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="31"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="54"/>
     </row>
     <row r="14" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
@@ -1116,33 +1116,33 @@
       <c r="B15" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="31"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="54"/>
     </row>
     <row r="16" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="47"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="49"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="51"/>
     </row>
     <row r="17" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="31"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="54"/>
     </row>
     <row r="18" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
@@ -1156,13 +1156,13 @@
       <c r="B19" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="31"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="54"/>
     </row>
     <row r="20" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
@@ -1176,13 +1176,13 @@
       <c r="B21" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="31"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="54"/>
     </row>
     <row r="22" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
@@ -1196,13 +1196,13 @@
       <c r="B23" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="31"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="54"/>
     </row>
     <row r="24" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
@@ -1218,21 +1218,21 @@
       <c r="B25" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="38" t="s">
+      <c r="C25" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="40"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="31"/>
     </row>
     <row r="26" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="43"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="34"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
@@ -1243,50 +1243,50 @@
       <c r="G27" s="6"/>
     </row>
     <row r="28" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="46"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="45"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="35"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="37"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="48"/>
     </row>
     <row r="30" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="50"/>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="49"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="51"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="38" t="s">
+      <c r="C31" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="40"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="31"/>
     </row>
     <row r="32" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="42"/>
-      <c r="G32" s="43"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="34"/>
     </row>
     <row r="33" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
@@ -1300,21 +1300,21 @@
       <c r="B34" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C34" s="38" t="s">
+      <c r="C34" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="40"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="31"/>
     </row>
     <row r="35" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="42"/>
-      <c r="G35" s="43"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="34"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
@@ -1325,22 +1325,22 @@
       <c r="G36" s="6"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="44" t="s">
+      <c r="B37" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="45"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="45"/>
-      <c r="G37" s="46"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="45"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="35"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="37"/>
+      <c r="B38" s="46"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="48"/>
     </row>
     <row r="39" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
@@ -1354,21 +1354,21 @@
       <c r="B40" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C40" s="38" t="s">
+      <c r="C40" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D40" s="39"/>
-      <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="40"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="31"/>
     </row>
     <row r="41" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
-      <c r="C41" s="41"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="42"/>
-      <c r="F41" s="42"/>
-      <c r="G41" s="43"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="34"/>
     </row>
     <row r="42" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
@@ -1382,312 +1382,320 @@
       <c r="B43" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C43" s="38" t="s">
+      <c r="C43" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D43" s="39"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="40"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="31"/>
     </row>
     <row r="44" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>
-      <c r="C44" s="41"/>
-      <c r="D44" s="42"/>
-      <c r="E44" s="42"/>
-      <c r="F44" s="42"/>
-      <c r="G44" s="43"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="33"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="34"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="51"/>
-      <c r="C45" s="52"/>
-      <c r="D45" s="52"/>
-      <c r="E45" s="52"/>
-      <c r="F45" s="52"/>
-      <c r="G45" s="53"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="41"/>
+      <c r="E45" s="41"/>
+      <c r="F45" s="41"/>
+      <c r="G45" s="42"/>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="44" t="s">
+      <c r="B46" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="C46" s="45"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="45"/>
-      <c r="F46" s="45"/>
-      <c r="G46" s="46"/>
+      <c r="C46" s="44"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="45"/>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="35"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="36"/>
-      <c r="E47" s="36"/>
-      <c r="F47" s="36"/>
-      <c r="G47" s="37"/>
+      <c r="B47" s="46"/>
+      <c r="C47" s="47"/>
+      <c r="D47" s="47"/>
+      <c r="E47" s="47"/>
+      <c r="F47" s="47"/>
+      <c r="G47" s="48"/>
     </row>
     <row r="48" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="51"/>
-      <c r="C48" s="52"/>
-      <c r="D48" s="52"/>
-      <c r="E48" s="52"/>
-      <c r="F48" s="52"/>
-      <c r="G48" s="53"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="41"/>
+      <c r="E48" s="41"/>
+      <c r="F48" s="41"/>
+      <c r="G48" s="42"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C49" s="38" t="s">
+      <c r="C49" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D49" s="39"/>
-      <c r="E49" s="39"/>
-      <c r="F49" s="39"/>
-      <c r="G49" s="40"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="30"/>
+      <c r="F49" s="30"/>
+      <c r="G49" s="31"/>
     </row>
     <row r="50" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="1"/>
-      <c r="C50" s="41"/>
-      <c r="D50" s="42"/>
-      <c r="E50" s="42"/>
-      <c r="F50" s="42"/>
-      <c r="G50" s="43"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="33"/>
+      <c r="E50" s="33"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="34"/>
     </row>
     <row r="51" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="51"/>
-      <c r="C51" s="52"/>
-      <c r="D51" s="52"/>
-      <c r="E51" s="52"/>
-      <c r="F51" s="52"/>
-      <c r="G51" s="53"/>
+      <c r="B51" s="40"/>
+      <c r="C51" s="41"/>
+      <c r="D51" s="41"/>
+      <c r="E51" s="41"/>
+      <c r="F51" s="41"/>
+      <c r="G51" s="42"/>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B52" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C52" s="38" t="s">
+      <c r="C52" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D52" s="39"/>
-      <c r="E52" s="39"/>
-      <c r="F52" s="39"/>
-      <c r="G52" s="40"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="30"/>
+      <c r="G52" s="31"/>
     </row>
     <row r="53" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="1"/>
-      <c r="C53" s="41"/>
-      <c r="D53" s="42"/>
-      <c r="E53" s="42"/>
-      <c r="F53" s="42"/>
-      <c r="G53" s="43"/>
+      <c r="C53" s="32"/>
+      <c r="D53" s="33"/>
+      <c r="E53" s="33"/>
+      <c r="F53" s="33"/>
+      <c r="G53" s="34"/>
     </row>
     <row r="54" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="51"/>
-      <c r="C54" s="52"/>
-      <c r="D54" s="52"/>
-      <c r="E54" s="52"/>
-      <c r="F54" s="52"/>
-      <c r="G54" s="53"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="41"/>
+      <c r="D54" s="41"/>
+      <c r="E54" s="41"/>
+      <c r="F54" s="41"/>
+      <c r="G54" s="42"/>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C55" s="38" t="s">
+      <c r="C55" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D55" s="39"/>
-      <c r="E55" s="39"/>
-      <c r="F55" s="39"/>
-      <c r="G55" s="40"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="30"/>
+      <c r="F55" s="30"/>
+      <c r="G55" s="31"/>
     </row>
     <row r="56" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="1"/>
-      <c r="C56" s="41"/>
-      <c r="D56" s="42"/>
-      <c r="E56" s="42"/>
-      <c r="F56" s="42"/>
-      <c r="G56" s="43"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="33"/>
+      <c r="E56" s="33"/>
+      <c r="F56" s="33"/>
+      <c r="G56" s="34"/>
     </row>
     <row r="57" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="51"/>
-      <c r="C57" s="52"/>
-      <c r="D57" s="52"/>
-      <c r="E57" s="52"/>
-      <c r="F57" s="52"/>
-      <c r="G57" s="53"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="41"/>
+      <c r="D57" s="41"/>
+      <c r="E57" s="41"/>
+      <c r="F57" s="41"/>
+      <c r="G57" s="42"/>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B58" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C58" s="38" t="s">
+      <c r="C58" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="D58" s="39"/>
-      <c r="E58" s="39"/>
-      <c r="F58" s="39"/>
-      <c r="G58" s="40"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="30"/>
+      <c r="F58" s="30"/>
+      <c r="G58" s="31"/>
     </row>
     <row r="59" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="1"/>
-      <c r="C59" s="41"/>
-      <c r="D59" s="42"/>
-      <c r="E59" s="42"/>
-      <c r="F59" s="42"/>
-      <c r="G59" s="43"/>
+      <c r="C59" s="32"/>
+      <c r="D59" s="33"/>
+      <c r="E59" s="33"/>
+      <c r="F59" s="33"/>
+      <c r="G59" s="34"/>
     </row>
     <row r="60" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="51"/>
-      <c r="C60" s="52"/>
-      <c r="D60" s="52"/>
-      <c r="E60" s="52"/>
-      <c r="F60" s="52"/>
-      <c r="G60" s="53"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="41"/>
+      <c r="D60" s="41"/>
+      <c r="E60" s="41"/>
+      <c r="F60" s="41"/>
+      <c r="G60" s="42"/>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B61" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C61" s="38" t="s">
+      <c r="C61" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D61" s="39"/>
-      <c r="E61" s="39"/>
-      <c r="F61" s="39"/>
-      <c r="G61" s="40"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="30"/>
+      <c r="F61" s="30"/>
+      <c r="G61" s="31"/>
     </row>
     <row r="62" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="1"/>
-      <c r="C62" s="41"/>
-      <c r="D62" s="42"/>
-      <c r="E62" s="42"/>
-      <c r="F62" s="42"/>
-      <c r="G62" s="43"/>
+      <c r="C62" s="32"/>
+      <c r="D62" s="33"/>
+      <c r="E62" s="33"/>
+      <c r="F62" s="33"/>
+      <c r="G62" s="34"/>
     </row>
     <row r="63" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="51"/>
-      <c r="C63" s="52"/>
-      <c r="D63" s="52"/>
-      <c r="E63" s="52"/>
-      <c r="F63" s="52"/>
-      <c r="G63" s="53"/>
+      <c r="B63" s="40"/>
+      <c r="C63" s="41"/>
+      <c r="D63" s="41"/>
+      <c r="E63" s="41"/>
+      <c r="F63" s="41"/>
+      <c r="G63" s="42"/>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B64" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C64" s="38" t="s">
+      <c r="C64" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D64" s="39"/>
-      <c r="E64" s="39"/>
-      <c r="F64" s="39"/>
-      <c r="G64" s="40"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="30"/>
+      <c r="G64" s="31"/>
     </row>
     <row r="65" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="1"/>
-      <c r="C65" s="41"/>
-      <c r="D65" s="42"/>
-      <c r="E65" s="42"/>
-      <c r="F65" s="42"/>
-      <c r="G65" s="43"/>
+      <c r="C65" s="32"/>
+      <c r="D65" s="33"/>
+      <c r="E65" s="33"/>
+      <c r="F65" s="33"/>
+      <c r="G65" s="34"/>
     </row>
     <row r="66" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="51"/>
-      <c r="C66" s="52"/>
-      <c r="D66" s="52"/>
-      <c r="E66" s="52"/>
-      <c r="F66" s="52"/>
-      <c r="G66" s="53"/>
+      <c r="B66" s="40"/>
+      <c r="C66" s="41"/>
+      <c r="D66" s="41"/>
+      <c r="E66" s="41"/>
+      <c r="F66" s="41"/>
+      <c r="G66" s="42"/>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C67" s="57" t="s">
+      <c r="C67" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="D67" s="39"/>
-      <c r="E67" s="39"/>
-      <c r="F67" s="39"/>
-      <c r="G67" s="40"/>
+      <c r="D67" s="30"/>
+      <c r="E67" s="30"/>
+      <c r="F67" s="30"/>
+      <c r="G67" s="31"/>
     </row>
     <row r="68" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="1"/>
-      <c r="C68" s="41"/>
-      <c r="D68" s="42"/>
-      <c r="E68" s="42"/>
-      <c r="F68" s="42"/>
-      <c r="G68" s="43"/>
+      <c r="C68" s="32"/>
+      <c r="D68" s="33"/>
+      <c r="E68" s="33"/>
+      <c r="F68" s="33"/>
+      <c r="G68" s="34"/>
     </row>
     <row r="69" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="51"/>
-      <c r="C69" s="52"/>
-      <c r="D69" s="52"/>
-      <c r="E69" s="52"/>
-      <c r="F69" s="52"/>
-      <c r="G69" s="53"/>
+      <c r="B69" s="40"/>
+      <c r="C69" s="41"/>
+      <c r="D69" s="41"/>
+      <c r="E69" s="41"/>
+      <c r="F69" s="41"/>
+      <c r="G69" s="42"/>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B70" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C70" s="38">
-        <v>2.11</v>
-      </c>
-      <c r="D70" s="39"/>
-      <c r="E70" s="39"/>
-      <c r="F70" s="39"/>
-      <c r="G70" s="40"/>
+      <c r="C70" s="29">
+        <v>4.7</v>
+      </c>
+      <c r="D70" s="30"/>
+      <c r="E70" s="30"/>
+      <c r="F70" s="30"/>
+      <c r="G70" s="31"/>
     </row>
     <row r="71" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="1"/>
-      <c r="C71" s="41"/>
-      <c r="D71" s="42"/>
-      <c r="E71" s="42"/>
-      <c r="F71" s="42"/>
-      <c r="G71" s="43"/>
+      <c r="C71" s="32"/>
+      <c r="D71" s="33"/>
+      <c r="E71" s="33"/>
+      <c r="F71" s="33"/>
+      <c r="G71" s="34"/>
     </row>
     <row r="72" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="54"/>
-      <c r="C72" s="55"/>
-      <c r="D72" s="55"/>
-      <c r="E72" s="55"/>
-      <c r="F72" s="55"/>
-      <c r="G72" s="56"/>
+      <c r="B72" s="35"/>
+      <c r="C72" s="36"/>
+      <c r="D72" s="36"/>
+      <c r="E72" s="36"/>
+      <c r="F72" s="36"/>
+      <c r="G72" s="37"/>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B73" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C73" s="57" t="s">
+      <c r="C73" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D73" s="58"/>
-      <c r="E73" s="58"/>
-      <c r="F73" s="58"/>
-      <c r="G73" s="58"/>
+      <c r="D73" s="39"/>
+      <c r="E73" s="39"/>
+      <c r="F73" s="39"/>
+      <c r="G73" s="39"/>
     </row>
     <row r="74" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="54"/>
-      <c r="C74" s="55"/>
-      <c r="D74" s="55"/>
-      <c r="E74" s="55"/>
-      <c r="F74" s="55"/>
-      <c r="G74" s="56"/>
+      <c r="B74" s="35"/>
+      <c r="C74" s="36"/>
+      <c r="D74" s="36"/>
+      <c r="E74" s="36"/>
+      <c r="F74" s="36"/>
+      <c r="G74" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="C70:G71"/>
-    <mergeCell ref="B72:G72"/>
-    <mergeCell ref="C73:G73"/>
-    <mergeCell ref="B74:G74"/>
-    <mergeCell ref="C61:G62"/>
-    <mergeCell ref="B63:G63"/>
-    <mergeCell ref="C64:G65"/>
-    <mergeCell ref="B66:G66"/>
-    <mergeCell ref="C67:G68"/>
-    <mergeCell ref="B69:G69"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="B1:G2"/>
+    <mergeCell ref="C4:G5"/>
+    <mergeCell ref="C7:G8"/>
+    <mergeCell ref="B10:G11"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C40:G41"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C25:G26"/>
+    <mergeCell ref="B28:G29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="C31:G32"/>
+    <mergeCell ref="C34:G35"/>
+    <mergeCell ref="B37:G38"/>
     <mergeCell ref="B60:G60"/>
     <mergeCell ref="C43:G44"/>
     <mergeCell ref="B45:G45"/>
@@ -1700,24 +1708,16 @@
     <mergeCell ref="C55:G56"/>
     <mergeCell ref="B57:G57"/>
     <mergeCell ref="C58:G59"/>
-    <mergeCell ref="C40:G41"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C25:G26"/>
-    <mergeCell ref="B28:G29"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="C31:G32"/>
-    <mergeCell ref="C34:G35"/>
-    <mergeCell ref="B37:G38"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="B1:G2"/>
-    <mergeCell ref="C4:G5"/>
-    <mergeCell ref="C7:G8"/>
-    <mergeCell ref="B10:G11"/>
-    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C70:G71"/>
+    <mergeCell ref="B72:G72"/>
+    <mergeCell ref="C73:G73"/>
+    <mergeCell ref="B74:G74"/>
+    <mergeCell ref="C61:G62"/>
+    <mergeCell ref="B63:G63"/>
+    <mergeCell ref="C64:G65"/>
+    <mergeCell ref="B66:G66"/>
+    <mergeCell ref="C67:G68"/>
+    <mergeCell ref="B69:G69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -1728,7 +1728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F40B79FA-81E3-4B65-BD43-437DAC09E605}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1882,9 +1882,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2091,27 +2094,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9798A1B8-6B7D-4E6C-A31B-78AFC6E86C13}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7B463CC-2C6E-4AEC-AFE4-31056C900892}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="0b7efa9e-1eed-4bd4-901e-1ea14744ffa0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="d82d40c8-bfdf-4ce1-b1ad-6594fbc9adc4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2136,9 +2127,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7B463CC-2C6E-4AEC-AFE4-31056C900892}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9798A1B8-6B7D-4E6C-A31B-78AFC6E86C13}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="0b7efa9e-1eed-4bd4-901e-1ea14744ffa0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="d82d40c8-bfdf-4ce1-b1ad-6594fbc9adc4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>